<commit_message>
Final Project Submission in Fulfillment of Requirements
</commit_message>
<xml_diff>
--- a/Resources/Final Logistic Regression Models.xlsx
+++ b/Resources/Final Logistic Regression Models.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://communsol-my.sharepoint.com/personal/judith_calvo_communitysolutions_org/Documents/_aUCB Data Analytics Bootcamp Class/Final Project Folder/ML/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judyc\OneDrive - Community Solutions\_aUCB Data Analytics Bootcamp Class\Final Project Folder\ML\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{E17BC8B0-290D-462B-AFC8-F01FB08EF523}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{341FDCAC-E622-4003-B4A0-5C1233205ED7}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{E17BC8B0-290D-462B-AFC8-F01FB08EF523}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E38712FB-95C6-442C-84A5-99AB0F3C993C}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
+    <workbookView xWindow="25700" yWindow="2660" windowWidth="17280" windowHeight="8980" firstSheet="5" activeTab="5" xr2:uid="{DE68D33D-2361-456F-8777-3D3631C620A9}"/>
   </bookViews>
   <sheets>
     <sheet name="data dictionary for Postgres" sheetId="1" r:id="rId1"/>
@@ -6212,7 +6212,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:G25"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -7422,18 +7422,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7456,26 +7456,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
-    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78112817-9362-4DB1-B53E-54BAB126672D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{571F5220-80D8-4F20-8AD7-DC1A6F626947}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b42430d8-c205-408e-a6b2-f7bcf1ddda46"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="076ed714-3a77-4f17-8bbf-04471c3fc2e1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>